<commit_message>
exclude covered calls when matching positions
</commit_message>
<xml_diff>
--- a/backtest results/Nifty covered call (monthly).xlsx
+++ b/backtest results/Nifty covered call (monthly).xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aniket.bhadane/Desktop/General/AniketBhadane.github.io/backtest results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B07568-99BD-A141-944A-6711EA91F3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA5C1C4-8452-394D-B0DB-0CC0F90196DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="month expiry to expiry" sheetId="4" r:id="rId1"/>
-    <sheet name="calendar month" sheetId="2" r:id="rId2"/>
+    <sheet name="month expiry to expiry - 300otm" sheetId="5" r:id="rId2"/>
+    <sheet name="calendar month" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="97">
   <si>
     <t>Date</t>
   </si>
@@ -313,6 +314,18 @@
   </si>
   <si>
     <t>close</t>
+  </si>
+  <si>
+    <t>call strike</t>
+  </si>
+  <si>
+    <t>call premium</t>
+  </si>
+  <si>
+    <t>atm call pnl</t>
+  </si>
+  <si>
+    <t>Strategy: Keep 300 pts difference. If spot is quite below, sell at the buying price of spot</t>
   </si>
 </sst>
 </file>
@@ -1278,6 +1291,513 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'month expiry to expiry - 300otm'!$J$2:$J$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-37.850000000000364</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-30.450000000000728</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-376.90000000000146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-558.15000000000146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-324.09999999999854</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-272.09999999999854</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-259.90000000000146</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-164.70000000000073</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4DE2-4E47-B978-2CBC5792A723}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'month expiry to expiry - 300otm'!$K$2:$K$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-37.850000000000364</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-190.45000000000073</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-536.90000000000146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-718.15000000000146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-384.09999999999854</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-272.09999999999854</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-359.90000000000146</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-164.70000000000073</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4DE2-4E47-B978-2CBC5792A723}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2018701344"/>
+        <c:axId val="2018648416"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2018701344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2018648416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2018648416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2018701344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:tx>
             <c:strRef>
               <c:f>'calendar month'!$J$1</c:f>
@@ -1664,6 +2184,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2168,6 +2728,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2712,6 +3775,47 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A536393-A269-E835-47C9-9B14B9A31DA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3051,8 +4155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EC9B32-201A-2948-B0D1-F0DBC04E9E60}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3154,7 +4258,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:K34" si="2">G3-I3</f>
+        <f t="shared" ref="J3:J34" si="2">G3-I3</f>
         <v>50</v>
       </c>
       <c r="L3" t="s">
@@ -4143,6 +5247,1235 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3996DEA-10BF-BC45-996B-A56CB4C67697}">
+  <dimension ref="A1:P41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2">
+        <v>15097.35</v>
+      </c>
+      <c r="E2">
+        <v>14324.9</v>
+      </c>
+      <c r="F2">
+        <v>15400</v>
+      </c>
+      <c r="G2">
+        <v>160</v>
+      </c>
+      <c r="H2">
+        <f>E2-F2</f>
+        <v>-1075.1000000000004</v>
+      </c>
+      <c r="I2">
+        <f>IF(H2&lt;0,0,H2)</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>G2-I2</f>
+        <v>160</v>
+      </c>
+      <c r="K2">
+        <v>300</v>
+      </c>
+      <c r="O2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2">
+        <f>COUNTIF($J$2:$J$200,"&gt;0")</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3">
+        <v>14324.9</v>
+      </c>
+      <c r="E3">
+        <v>14894.9</v>
+      </c>
+      <c r="F3">
+        <v>15100</v>
+      </c>
+      <c r="G3">
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H34" si="0">E3-F3</f>
+        <v>-205.10000000000036</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I34" si="1">IF(H3&lt;0,0,H3)</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J34" si="2">G3-I3</f>
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <v>50</v>
+      </c>
+      <c r="O3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3">
+        <f>COUNTIF($J$2:$J$200,"&lt;=0")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4">
+        <v>14894.9</v>
+      </c>
+      <c r="E4">
+        <v>15337.85</v>
+      </c>
+      <c r="F4">
+        <v>15100</v>
+      </c>
+      <c r="G4">
+        <v>200</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>237.85000000000036</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>237.85000000000036</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>-37.850000000000364</v>
+      </c>
+      <c r="K4">
+        <v>-37.850000000000364</v>
+      </c>
+      <c r="O4" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" s="1">
+        <f>P2/(P2+P3)</f>
+        <v>0.76470588235294112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <v>15337.85</v>
+      </c>
+      <c r="E5">
+        <v>15790.45</v>
+      </c>
+      <c r="F5">
+        <v>15600</v>
+      </c>
+      <c r="G5">
+        <v>160</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>190.45000000000073</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>190.45000000000073</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>-30.450000000000728</v>
+      </c>
+      <c r="K5">
+        <v>-190.45000000000073</v>
+      </c>
+      <c r="O5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P5" s="2">
+        <f>100%-P4</f>
+        <v>0.23529411764705888</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>15790.45</v>
+      </c>
+      <c r="E6">
+        <v>15778.45</v>
+      </c>
+      <c r="F6">
+        <v>16100</v>
+      </c>
+      <c r="G6">
+        <v>160</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>-321.54999999999927</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="K6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>15778.45</v>
+      </c>
+      <c r="E7">
+        <v>16636.900000000001</v>
+      </c>
+      <c r="F7">
+        <v>16100</v>
+      </c>
+      <c r="G7">
+        <v>160</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>536.90000000000146</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>536.90000000000146</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>-376.90000000000146</v>
+      </c>
+      <c r="K7">
+        <v>-536.90000000000146</v>
+      </c>
+      <c r="O7" t="s">
+        <v>47</v>
+      </c>
+      <c r="P7" s="3">
+        <f>AVERAGEIF($J$2:$J$200,"&gt;0")</f>
+        <v>102.1480769230768</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8">
+        <v>16636.900000000001</v>
+      </c>
+      <c r="E8">
+        <v>17618.150000000001</v>
+      </c>
+      <c r="F8">
+        <v>16900</v>
+      </c>
+      <c r="G8">
+        <v>160</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>718.15000000000146</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>718.15000000000146</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>-558.15000000000146</v>
+      </c>
+      <c r="K8">
+        <v>-718.15000000000146</v>
+      </c>
+      <c r="O8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P8" s="3">
+        <f>AVERAGEIF($J$2:$J$200,"&lt;=0")</f>
+        <v>-253.01875000000041</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9">
+        <v>17618.150000000001</v>
+      </c>
+      <c r="E9">
+        <v>17857.25</v>
+      </c>
+      <c r="F9">
+        <v>17900</v>
+      </c>
+      <c r="G9">
+        <v>160</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>-42.75</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="K9">
+        <v>42.75</v>
+      </c>
+      <c r="O9" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" s="3">
+        <f>P7/ABS(P8)</f>
+        <v>0.4037174198476462</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10">
+        <v>17857.25</v>
+      </c>
+      <c r="E10">
+        <v>17536.25</v>
+      </c>
+      <c r="F10">
+        <v>18100</v>
+      </c>
+      <c r="G10">
+        <v>160</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>-563.75</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="K10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <v>17536.25</v>
+      </c>
+      <c r="E11">
+        <v>17203.95</v>
+      </c>
+      <c r="F11">
+        <v>17800</v>
+      </c>
+      <c r="G11">
+        <v>200</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>-596.04999999999927</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="K11">
+        <v>200</v>
+      </c>
+      <c r="O11" t="s">
+        <v>50</v>
+      </c>
+      <c r="P11">
+        <f>MAX($J$2:$J$200)</f>
+        <v>315.84999999999673</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12">
+        <v>17203.95</v>
+      </c>
+      <c r="E12">
+        <v>17110.150000000001</v>
+      </c>
+      <c r="F12">
+        <v>17800</v>
+      </c>
+      <c r="G12">
+        <v>60</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>-689.84999999999854</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="K12">
+        <v>60</v>
+      </c>
+      <c r="O12" t="s">
+        <v>51</v>
+      </c>
+      <c r="P12">
+        <f>MIN($J$2:$J$200)</f>
+        <v>-558.15000000000146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13">
+        <v>17110.150000000001</v>
+      </c>
+      <c r="E13">
+        <v>16247.95</v>
+      </c>
+      <c r="F13">
+        <v>17800</v>
+      </c>
+      <c r="G13">
+        <v>40</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>-1552.0499999999993</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="K13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14">
+        <v>16247.95</v>
+      </c>
+      <c r="E14">
+        <v>17222.75</v>
+      </c>
+      <c r="F14">
+        <v>17800</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>-577.25</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="O14" t="s">
+        <v>52</v>
+      </c>
+      <c r="P14" s="3">
+        <f>(P4*P7)+(P5*P8)</f>
+        <v>18.579411764705668</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15">
+        <v>17222.75</v>
+      </c>
+      <c r="E15">
+        <v>17245.05</v>
+      </c>
+      <c r="F15">
+        <v>17800</v>
+      </c>
+      <c r="G15">
+        <v>60</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>-554.95000000000073</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="K15">
+        <v>60</v>
+      </c>
+      <c r="O15" t="s">
+        <v>53</v>
+      </c>
+      <c r="P15" s="3">
+        <f>(P9*P4)-P5</f>
+        <v>7.3430968118788187E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16">
+        <v>17245.05</v>
+      </c>
+      <c r="E16">
+        <v>16170.15</v>
+      </c>
+      <c r="F16">
+        <v>17800</v>
+      </c>
+      <c r="G16">
+        <v>60</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>-1629.8500000000004</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="K16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>16170.15</v>
+      </c>
+      <c r="E17">
+        <v>15780.25</v>
+      </c>
+      <c r="F17">
+        <v>17800</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>-2019.75</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="K17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18">
+        <v>15780.25</v>
+      </c>
+      <c r="E18">
+        <v>16929.599999999999</v>
+      </c>
+      <c r="F18">
+        <v>17800</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>-870.40000000000146</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <v>16929.599999999999</v>
+      </c>
+      <c r="E19">
+        <v>17522.45</v>
+      </c>
+      <c r="F19">
+        <v>17800</v>
+      </c>
+      <c r="G19">
+        <v>30</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>-277.54999999999927</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="K19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20">
+        <v>17522.45</v>
+      </c>
+      <c r="E20">
+        <v>16818.099999999999</v>
+      </c>
+      <c r="F20">
+        <v>17800</v>
+      </c>
+      <c r="G20">
+        <v>200</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>-981.90000000000146</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="K20">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21">
+        <v>16818.099999999999</v>
+      </c>
+      <c r="E21">
+        <v>17736.95</v>
+      </c>
+      <c r="F21">
+        <v>17800</v>
+      </c>
+      <c r="G21">
+        <v>15</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>-63.049999999999272</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="K21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22">
+        <v>17736.95</v>
+      </c>
+      <c r="E22">
+        <v>18484.099999999999</v>
+      </c>
+      <c r="F22">
+        <v>18000</v>
+      </c>
+      <c r="G22">
+        <v>160</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>484.09999999999854</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>484.09999999999854</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>-324.09999999999854</v>
+      </c>
+      <c r="K22">
+        <v>-384.09999999999854</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23">
+        <v>18484.099999999999</v>
+      </c>
+      <c r="E23">
+        <v>18191</v>
+      </c>
+      <c r="F23">
+        <v>18700</v>
+      </c>
+      <c r="G23">
+        <v>200</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>-509</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="K23">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24">
+        <v>18191</v>
+      </c>
+      <c r="E24">
+        <v>17891.95</v>
+      </c>
+      <c r="F24">
+        <v>18500</v>
+      </c>
+      <c r="G24">
+        <v>150</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>-608.04999999999927</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="K24">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25">
+        <v>17891.95</v>
+      </c>
+      <c r="E25">
+        <v>17511.25</v>
+      </c>
+      <c r="F25">
+        <v>18500</v>
+      </c>
+      <c r="G25">
+        <v>60</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>-988.75</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="K25">
+        <v>60</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26">
+        <v>17511.25</v>
+      </c>
+      <c r="E26">
+        <v>17080.7</v>
+      </c>
+      <c r="F26">
+        <v>18500</v>
+      </c>
+      <c r="G26">
+        <v>15</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>-1419.2999999999993</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="K26">
+        <v>15</v>
+      </c>
+      <c r="O26">
+        <v>100</v>
+      </c>
+      <c r="P26">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27">
+        <v>17080.7</v>
+      </c>
+      <c r="E27">
+        <v>17915.05</v>
+      </c>
+      <c r="F27">
+        <v>18500</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>-584.95000000000073</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="K27">
+        <v>5</v>
+      </c>
+      <c r="O27">
+        <v>200</v>
+      </c>
+      <c r="P27">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28">
+        <v>17915.05</v>
+      </c>
+      <c r="E28">
+        <v>18321.150000000001</v>
+      </c>
+      <c r="F28">
+        <v>18500</v>
+      </c>
+      <c r="G28">
+        <v>60</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>-178.84999999999854</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="K28">
+        <v>60</v>
+      </c>
+      <c r="O28">
+        <v>300</v>
+      </c>
+      <c r="P28">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29">
+        <v>18321.150000000001</v>
+      </c>
+      <c r="E29">
+        <v>18972.099999999999</v>
+      </c>
+      <c r="F29">
+        <v>18500</v>
+      </c>
+      <c r="G29">
+        <v>200</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>472.09999999999854</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>472.09999999999854</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>-272.09999999999854</v>
+      </c>
+      <c r="K29">
+        <v>-272.09999999999854</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30">
+        <v>18972.099999999999</v>
+      </c>
+      <c r="E30">
+        <v>19659.900000000001</v>
+      </c>
+      <c r="F30">
+        <v>19200</v>
+      </c>
+      <c r="G30">
+        <v>200</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>459.90000000000146</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>459.90000000000146</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="2"/>
+        <v>-259.90000000000146</v>
+      </c>
+      <c r="K30">
+        <v>-359.90000000000146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31">
+        <v>19659.900000000001</v>
+      </c>
+      <c r="E31">
+        <v>19253.8</v>
+      </c>
+      <c r="F31">
+        <v>19900</v>
+      </c>
+      <c r="G31">
+        <v>200</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>-646.20000000000073</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="K31">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32">
+        <v>19253.8</v>
+      </c>
+      <c r="E32">
+        <v>19523.55</v>
+      </c>
+      <c r="F32">
+        <v>19600</v>
+      </c>
+      <c r="G32">
+        <v>120</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>-76.450000000000728</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="K32">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33">
+        <v>19523.55</v>
+      </c>
+      <c r="E33">
+        <v>18857.25</v>
+      </c>
+      <c r="F33">
+        <v>19800</v>
+      </c>
+      <c r="G33">
+        <v>160</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>-942.75</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="K33">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34">
+        <v>18857.25</v>
+      </c>
+      <c r="E34">
+        <v>19794.7</v>
+      </c>
+      <c r="F34">
+        <v>19600</v>
+      </c>
+      <c r="G34">
+        <v>30</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>194.70000000000073</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>194.70000000000073</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="2"/>
+        <v>-164.70000000000073</v>
+      </c>
+      <c r="K34">
+        <v>-164.70000000000073</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I35" t="s">
+        <v>54</v>
+      </c>
+      <c r="J35">
+        <f>SUM(J2:J34)</f>
+        <v>315.84999999999673</v>
+      </c>
+      <c r="K35">
+        <v>318.59999999999673</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M35"/>
   <sheetViews>

</xml_diff>

<commit_message>
increase days to retrieve for exporting expiry data
</commit_message>
<xml_diff>
--- a/backtest results/Nifty covered call (monthly).xlsx
+++ b/backtest results/Nifty covered call (monthly).xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aniket.bhadane/Desktop/General/AniketBhadane.github.io/backtest results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A949513A-42A2-9F4B-AD4B-163EDDA90963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C507FD-4AE7-6146-B3CB-E7CAB1C17304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="month expiry to expiry" sheetId="4" r:id="rId1"/>
-    <sheet name="month expiry - always ATM" sheetId="6" r:id="rId2"/>
-    <sheet name="month expiry to expiry - 300otm" sheetId="5" r:id="rId3"/>
-    <sheet name="calendar month" sheetId="2" r:id="rId4"/>
-    <sheet name="open close" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
+    <sheet name="month expiry - always ATM" sheetId="6" r:id="rId3"/>
+    <sheet name="month expiry to expiry - 300otm" sheetId="5" r:id="rId4"/>
+    <sheet name="calendar month" sheetId="2" r:id="rId5"/>
+    <sheet name="open close" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'open close'!$A$1:$A$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'open close'!$A$1:$A$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="99">
   <si>
     <t>Date</t>
   </si>
@@ -334,6 +335,9 @@
   </si>
   <si>
     <t>cumulative</t>
+  </si>
+  <si>
+    <t>cum pnl</t>
   </si>
 </sst>
 </file>
@@ -1653,6 +1657,367 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'month expiry to expiry'!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cum pnl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'month expiry to expiry'!$L$2:$L$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>-472.45000000000073</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>147.54999999999927</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>552.64999999999964</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>814.79999999999927</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1102.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1424.3499999999967</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1687.4499999999953</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1969.2999999999938</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1948.2999999999938</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1815.9999999999982</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1782.1999999999953</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>959.99999999999636</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1939.7999999999938</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2022.0999999999967</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1007.1999999999953</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>622.29999999999563</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1776.6499999999924</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2399.4999999999982</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1895.1499999999924</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2828.9999999999982</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3192.0499999999938</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3198.9499999999953</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3049.8999999999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2729.1999999999953</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2313.6499999999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3152.9999999999982</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3619.0999999999967</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3997.9499999999953</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4325.8499999999967</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4219.7499999999982</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4609.4999999999982</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4243.1999999999953</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5015.9499999999953</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-98C7-5F46-86EC-FABBED7A2020}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="429499999"/>
+        <c:axId val="1258094591"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="429499999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1258094591"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1258094591"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="429499999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1969,7 +2334,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -2476,7 +2841,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -2836,7 +3201,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -3436,6 +3801,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4456,7 +4861,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4564,6 +4969,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -4574,6 +4984,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -4605,6 +5020,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6467,20 +6885,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>82550</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6507,16 +7428,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>450850</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6536,6 +7457,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BC9D1BB-297A-DF80-8E03-A53EC8C487C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7007,10 +7964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EC9B32-201A-2948-B0D1-F0DBC04E9E60}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7019,7 +7976,7 @@
     <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -7053,8 +8010,11 @@
       <c r="K1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -7086,15 +8046,19 @@
         <f>J2</f>
         <v>300</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2">
+        <f>K2+E2-$B$2</f>
+        <v>-472.45000000000073</v>
+      </c>
+      <c r="M2" t="s">
         <v>43</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <f>COUNTIF($J$2:$J$200,"&gt;0")</f>
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -7126,15 +8090,19 @@
         <f>J3+K2</f>
         <v>350</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3">
+        <f t="shared" ref="L3:L34" si="3">K3+E3-$B$2</f>
+        <v>147.54999999999927</v>
+      </c>
+      <c r="M3" t="s">
         <v>44</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <f>COUNTIF($J$2:$J$200,"&lt;=0")</f>
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -7163,18 +8131,22 @@
         <v>-37.850000000000364</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K34" si="3">J4+K3</f>
+        <f t="shared" ref="K4:K34" si="4">J4+K3</f>
         <v>312.14999999999964</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>552.64999999999964</v>
+      </c>
+      <c r="M4" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="1">
-        <f>M2/(M2+M3)</f>
+      <c r="N4" s="1">
+        <f>N2/(N2+N3)</f>
         <v>0.76470588235294112</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -7203,18 +8175,22 @@
         <v>-190.45000000000073</v>
       </c>
       <c r="K5">
+        <f t="shared" si="4"/>
+        <v>121.69999999999891</v>
+      </c>
+      <c r="L5">
         <f t="shared" si="3"/>
-        <v>121.69999999999891</v>
-      </c>
-      <c r="L5" t="s">
+        <v>814.79999999999927</v>
+      </c>
+      <c r="M5" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="2">
-        <f>100%-M4</f>
+      <c r="N5" s="2">
+        <f>100%-N4</f>
         <v>0.23529411764705888</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -7243,11 +8219,15 @@
         <v>300</v>
       </c>
       <c r="K6">
+        <f t="shared" si="4"/>
+        <v>421.69999999999891</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="3"/>
-        <v>421.69999999999891</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1102.7999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -7276,18 +8256,22 @@
         <v>-536.90000000000146</v>
       </c>
       <c r="K7">
+        <f t="shared" si="4"/>
+        <v>-115.20000000000255</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="3"/>
-        <v>-115.20000000000255</v>
-      </c>
-      <c r="L7" t="s">
+        <v>1424.3499999999967</v>
+      </c>
+      <c r="M7" t="s">
         <v>47</v>
       </c>
-      <c r="M7" s="3">
+      <c r="N7" s="3">
         <f>AVERAGEIF($J$2:$J$200,"&gt;0")</f>
         <v>126.97499999999988</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -7316,18 +8300,22 @@
         <v>-718.15000000000146</v>
       </c>
       <c r="K8">
+        <f t="shared" si="4"/>
+        <v>-833.350000000004</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="3"/>
-        <v>-833.350000000004</v>
-      </c>
-      <c r="L8" t="s">
+        <v>1687.4499999999953</v>
+      </c>
+      <c r="M8" t="s">
         <v>48</v>
       </c>
-      <c r="M8" s="3">
+      <c r="N8" s="3">
         <f>AVERAGEIF($J$2:$J$200,"&lt;=0")</f>
         <v>-333.01875000000041</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -7356,18 +8344,22 @@
         <v>42.75</v>
       </c>
       <c r="K9">
+        <f t="shared" si="4"/>
+        <v>-790.600000000004</v>
+      </c>
+      <c r="L9">
         <f t="shared" si="3"/>
-        <v>-790.600000000004</v>
-      </c>
-      <c r="L9" t="s">
+        <v>1969.2999999999938</v>
+      </c>
+      <c r="M9" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="3">
-        <f>M7/ABS(M8)</f>
+      <c r="N9" s="3">
+        <f>N7/ABS(N8)</f>
         <v>0.38128483756545156</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -7396,11 +8388,15 @@
         <v>300</v>
       </c>
       <c r="K10">
+        <f t="shared" si="4"/>
+        <v>-490.600000000004</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="3"/>
-        <v>-490.600000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1948.2999999999938</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -7429,18 +8425,22 @@
         <v>200</v>
       </c>
       <c r="K11">
+        <f t="shared" si="4"/>
+        <v>-290.600000000004</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="3"/>
-        <v>-290.600000000004</v>
-      </c>
-      <c r="L11" t="s">
+        <v>1815.9999999999982</v>
+      </c>
+      <c r="M11" t="s">
         <v>50</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <f>MAX($J$2:$J$200)</f>
         <v>318.59999999999673</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -7469,18 +8469,22 @@
         <v>60</v>
       </c>
       <c r="K12">
+        <f t="shared" si="4"/>
+        <v>-230.600000000004</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="3"/>
-        <v>-230.600000000004</v>
-      </c>
-      <c r="L12" t="s">
+        <v>1782.1999999999953</v>
+      </c>
+      <c r="M12" t="s">
         <v>51</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <f>MIN($J$2:$J$200)</f>
         <v>-718.15000000000146</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -7509,11 +8513,15 @@
         <v>40</v>
       </c>
       <c r="K13">
+        <f t="shared" si="4"/>
+        <v>-190.600000000004</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="3"/>
-        <v>-190.600000000004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>959.99999999999636</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -7542,18 +8550,22 @@
         <v>5</v>
       </c>
       <c r="K14">
+        <f t="shared" si="4"/>
+        <v>-185.600000000004</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="3"/>
-        <v>-185.600000000004</v>
-      </c>
-      <c r="L14" t="s">
+        <v>1939.7999999999938</v>
+      </c>
+      <c r="M14" t="s">
         <v>52</v>
       </c>
-      <c r="M14" s="3">
-        <f>(M4*M7)+(M5*M8)</f>
+      <c r="N14" s="3">
+        <f>(N4*N7)+(N5*N8)</f>
         <v>18.741176470588016</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -7582,18 +8594,22 @@
         <v>60</v>
       </c>
       <c r="K15">
+        <f t="shared" si="4"/>
+        <v>-125.600000000004</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="3"/>
-        <v>-125.600000000004</v>
-      </c>
-      <c r="L15" t="s">
+        <v>2022.0999999999967</v>
+      </c>
+      <c r="M15" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="3">
-        <f>(M9*M4)-M5</f>
+      <c r="N15" s="3">
+        <f>(N9*N4)-N5</f>
         <v>5.6276640491227603E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -7622,11 +8638,15 @@
         <v>60</v>
       </c>
       <c r="K16">
+        <f t="shared" si="4"/>
+        <v>-65.600000000004002</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="3"/>
-        <v>-65.600000000004002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1007.1999999999953</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -7655,11 +8675,15 @@
         <v>5</v>
       </c>
       <c r="K17">
+        <f t="shared" si="4"/>
+        <v>-60.600000000004002</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="3"/>
-        <v>-60.600000000004002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+        <v>622.29999999999563</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -7688,11 +8712,15 @@
         <v>5</v>
       </c>
       <c r="K18">
+        <f t="shared" si="4"/>
+        <v>-55.600000000004002</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="3"/>
-        <v>-55.600000000004002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1776.6499999999924</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -7721,11 +8749,15 @@
         <v>30</v>
       </c>
       <c r="K19">
+        <f t="shared" si="4"/>
+        <v>-25.600000000004002</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="3"/>
-        <v>-25.600000000004002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2399.4999999999982</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -7754,11 +8786,15 @@
         <v>200</v>
       </c>
       <c r="K20">
+        <f t="shared" si="4"/>
+        <v>174.399999999996</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="3"/>
-        <v>174.399999999996</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1895.1499999999924</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -7787,11 +8823,15 @@
         <v>15</v>
       </c>
       <c r="K21">
+        <f t="shared" si="4"/>
+        <v>189.399999999996</v>
+      </c>
+      <c r="L21">
         <f t="shared" si="3"/>
-        <v>189.399999999996</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2828.9999999999982</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -7820,11 +8860,15 @@
         <v>-384.09999999999854</v>
       </c>
       <c r="K22">
+        <f t="shared" si="4"/>
+        <v>-194.70000000000255</v>
+      </c>
+      <c r="L22">
         <f t="shared" si="3"/>
-        <v>-194.70000000000255</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3192.0499999999938</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -7853,11 +8897,15 @@
         <v>300</v>
       </c>
       <c r="K23">
+        <f t="shared" si="4"/>
+        <v>105.29999999999745</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="3"/>
-        <v>105.29999999999745</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3198.9499999999953</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -7886,11 +8934,15 @@
         <v>150</v>
       </c>
       <c r="K24">
+        <f t="shared" si="4"/>
+        <v>255.29999999999745</v>
+      </c>
+      <c r="L24">
         <f t="shared" si="3"/>
-        <v>255.29999999999745</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3049.8999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -7919,11 +8971,15 @@
         <v>60</v>
       </c>
       <c r="K25">
+        <f t="shared" si="4"/>
+        <v>315.29999999999745</v>
+      </c>
+      <c r="L25">
         <f t="shared" si="3"/>
-        <v>315.29999999999745</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2729.1999999999953</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -7952,11 +9008,15 @@
         <v>15</v>
       </c>
       <c r="K26">
+        <f t="shared" si="4"/>
+        <v>330.29999999999745</v>
+      </c>
+      <c r="L26">
         <f t="shared" si="3"/>
-        <v>330.29999999999745</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2313.6499999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -7985,11 +9045,15 @@
         <v>5</v>
       </c>
       <c r="K27">
+        <f t="shared" si="4"/>
+        <v>335.29999999999745</v>
+      </c>
+      <c r="L27">
         <f t="shared" si="3"/>
-        <v>335.29999999999745</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3152.9999999999982</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -8018,11 +9082,15 @@
         <v>60</v>
       </c>
       <c r="K28">
+        <f t="shared" si="4"/>
+        <v>395.29999999999745</v>
+      </c>
+      <c r="L28">
         <f t="shared" si="3"/>
-        <v>395.29999999999745</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3619.0999999999967</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -8051,11 +9119,15 @@
         <v>-272.09999999999854</v>
       </c>
       <c r="K29">
+        <f t="shared" si="4"/>
+        <v>123.19999999999891</v>
+      </c>
+      <c r="L29">
         <f t="shared" si="3"/>
-        <v>123.19999999999891</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3997.9499999999953</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>83</v>
       </c>
@@ -8084,11 +9156,15 @@
         <v>-359.90000000000146</v>
       </c>
       <c r="K30">
+        <f t="shared" si="4"/>
+        <v>-236.70000000000255</v>
+      </c>
+      <c r="L30">
         <f t="shared" si="3"/>
-        <v>-236.70000000000255</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+        <v>4325.8499999999967</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -8117,11 +9193,15 @@
         <v>300</v>
       </c>
       <c r="K31">
+        <f t="shared" si="4"/>
+        <v>63.299999999997453</v>
+      </c>
+      <c r="L31">
         <f t="shared" si="3"/>
-        <v>63.299999999997453</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+        <v>4219.7499999999982</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -8150,11 +9230,15 @@
         <v>120</v>
       </c>
       <c r="K32">
+        <f t="shared" si="4"/>
+        <v>183.29999999999745</v>
+      </c>
+      <c r="L32">
         <f t="shared" si="3"/>
-        <v>183.29999999999745</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+        <v>4609.4999999999982</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -8183,11 +9267,15 @@
         <v>300</v>
       </c>
       <c r="K33">
+        <f t="shared" si="4"/>
+        <v>483.29999999999745</v>
+      </c>
+      <c r="L33">
         <f t="shared" si="3"/>
-        <v>483.29999999999745</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+        <v>4243.1999999999953</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>87</v>
       </c>
@@ -8216,11 +9304,15 @@
         <v>-164.70000000000073</v>
       </c>
       <c r="K34">
+        <f t="shared" si="4"/>
+        <v>318.59999999999673</v>
+      </c>
+      <c r="L34">
         <f t="shared" si="3"/>
-        <v>318.59999999999673</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+        <v>5015.9499999999953</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I35" t="s">
         <v>54</v>
       </c>
@@ -8236,6 +9328,431 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DC62E7A-1A37-CF4F-82A8-99FEDF35032D}">
+  <dimension ref="A1:E34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="A16:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>15097.35</v>
+      </c>
+      <c r="D2">
+        <v>14324.9</v>
+      </c>
+      <c r="E2">
+        <f>D2-A2</f>
+        <v>-772.45000000000073</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>14324.9</v>
+      </c>
+      <c r="D3">
+        <v>14894.9</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E34" si="0">D3-A3</f>
+        <v>570</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>14894.9</v>
+      </c>
+      <c r="D4">
+        <v>15337.85</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>442.95000000000073</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>15337.85</v>
+      </c>
+      <c r="D5">
+        <v>15790.45</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>452.60000000000036</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>15790.45</v>
+      </c>
+      <c r="D6">
+        <v>15778.45</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>15778.45</v>
+      </c>
+      <c r="D7">
+        <v>16636.900000000001</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>858.45000000000073</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16636.900000000001</v>
+      </c>
+      <c r="D8">
+        <v>17618.150000000001</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>981.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>17618.150000000001</v>
+      </c>
+      <c r="D9">
+        <v>17857.25</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>239.09999999999854</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>17857.25</v>
+      </c>
+      <c r="D10">
+        <v>17536.25</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>-321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>17536.25</v>
+      </c>
+      <c r="D11">
+        <v>17203.95</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>-332.29999999999927</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>17203.95</v>
+      </c>
+      <c r="D12">
+        <v>17110.150000000001</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>-93.799999999999272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>17110.150000000001</v>
+      </c>
+      <c r="D13">
+        <v>16247.95</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>-862.20000000000073</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>16247.95</v>
+      </c>
+      <c r="D14">
+        <v>17222.75</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>974.79999999999927</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>17222.75</v>
+      </c>
+      <c r="D15">
+        <v>17245.05</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>22.299999999999272</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>17245.05</v>
+      </c>
+      <c r="D16">
+        <v>16170.15</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>-1074.8999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16170.15</v>
+      </c>
+      <c r="D17">
+        <v>15780.25</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>-389.89999999999964</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>15780.25</v>
+      </c>
+      <c r="D18">
+        <v>16929.599999999999</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1149.3499999999985</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>16929.599999999999</v>
+      </c>
+      <c r="D19">
+        <v>17522.45</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>592.85000000000218</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>17522.45</v>
+      </c>
+      <c r="D20">
+        <v>16818.099999999999</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>-704.35000000000218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>16818.099999999999</v>
+      </c>
+      <c r="D21">
+        <v>17736.95</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>918.85000000000218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>17736.95</v>
+      </c>
+      <c r="D22">
+        <v>18484.099999999999</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>747.14999999999782</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>18484.099999999999</v>
+      </c>
+      <c r="D23">
+        <v>18191</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>-293.09999999999854</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>18191</v>
+      </c>
+      <c r="D24">
+        <v>17891.95</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>-299.04999999999927</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>17891.95</v>
+      </c>
+      <c r="D25">
+        <v>17511.25</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>-380.70000000000073</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>17511.25</v>
+      </c>
+      <c r="D26">
+        <v>17080.7</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>-430.54999999999927</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>17080.7</v>
+      </c>
+      <c r="D27">
+        <v>17915.05</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>834.34999999999854</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>17915.05</v>
+      </c>
+      <c r="D28">
+        <v>18321.150000000001</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>406.10000000000218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>18321.150000000001</v>
+      </c>
+      <c r="D29">
+        <v>18972.099999999999</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>650.94999999999709</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>18972.099999999999</v>
+      </c>
+      <c r="D30">
+        <v>19659.900000000001</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>687.80000000000291</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>19659.900000000001</v>
+      </c>
+      <c r="D31">
+        <v>19253.8</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>-406.10000000000218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>19253.8</v>
+      </c>
+      <c r="D32">
+        <v>19523.55</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>269.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>19523.55</v>
+      </c>
+      <c r="D33">
+        <v>18857.25</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>-666.29999999999927</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>18857.25</v>
+      </c>
+      <c r="D34">
+        <v>19794.7</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>937.45000000000073</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE79CB69-617B-754A-A584-16FD5CFFED71}">
   <dimension ref="A1:M35"/>
   <sheetViews>
@@ -9330,7 +10847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3996DEA-10BF-BC45-996B-A56CB4C67697}">
   <dimension ref="A1:P41"/>
   <sheetViews>
@@ -10559,7 +12076,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M35"/>
   <sheetViews>
@@ -11851,7 +13368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{573F8634-9262-464A-A186-58DAA03B4997}">
   <dimension ref="A1:A34"/>
   <sheetViews>

</xml_diff>